<commit_message>
update dashboard.py - ubah kolom klasifikasi - ubah kolom exel lasifikasi data 1
</commit_message>
<xml_diff>
--- a/keterangan DDC.xlsx
+++ b/keterangan DDC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data percobaan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANIS SKRIPSI\KNN3\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D14EC6-E452-4641-A613-E587F961D689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3873046C-8EC9-4EA4-B0A3-EED7C49FF37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{0BBDD3C5-C6DD-47CE-9848-CA545DA301BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{0BBDD3C5-C6DD-47CE-9848-CA545DA301BC}"/>
   </bookViews>
   <sheets>
     <sheet name="data 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>Klasifikasi</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Statistik</t>
-  </si>
-  <si>
-    <t>Klasifikasi level 2</t>
   </si>
   <si>
     <t>Ensiklopedi Umum</t>
@@ -679,9 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC40BA6-2FCC-471D-9419-3917E1936DCD}">
   <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -691,7 +686,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -738,7 +733,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2">
         <v>2</v>
@@ -749,7 +744,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -760,7 +755,7 @@
         <v>60</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -771,7 +766,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -782,7 +777,7 @@
         <v>100</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2">
         <v>5</v>
@@ -793,7 +788,7 @@
         <v>110</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2">
         <v>6</v>
@@ -804,7 +799,7 @@
         <v>120</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2">
         <v>6</v>
@@ -815,7 +810,7 @@
         <v>130</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -837,7 +832,7 @@
         <v>160</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2">
         <v>3</v>
@@ -859,7 +854,7 @@
         <v>180</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2">
         <v>2</v>
@@ -881,7 +876,7 @@
         <v>220</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
@@ -892,7 +887,7 @@
         <v>230</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
@@ -903,7 +898,7 @@
         <v>250</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="2">
         <v>2</v>
@@ -1046,7 +1041,7 @@
         <v>410</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="2">
         <v>6</v>
@@ -1068,7 +1063,7 @@
         <v>430</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="2">
         <v>3</v>
@@ -1079,7 +1074,7 @@
         <v>440</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="2">
         <v>2</v>
@@ -1112,7 +1107,7 @@
         <v>520</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="2">
         <v>6</v>
@@ -1299,7 +1294,7 @@
         <v>700</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C56" s="2">
         <v>6</v>
@@ -1310,7 +1305,7 @@
         <v>710</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C57" s="2">
         <v>2</v>
@@ -1398,7 +1393,7 @@
         <v>830</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C65" s="2">
         <v>3</v>
@@ -1409,7 +1404,7 @@
         <v>850</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C66" s="2">
         <v>1</v>
@@ -1420,7 +1415,7 @@
         <v>880</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C67" s="2">
         <v>3</v>
@@ -1442,7 +1437,7 @@
         <v>900</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="2">
         <v>4</v>
@@ -1475,7 +1470,7 @@
         <v>930</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72" s="2">
         <v>7</v>
@@ -1486,7 +1481,7 @@
         <v>950</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C73" s="2">
         <v>2</v>
@@ -1497,7 +1492,7 @@
         <v>980</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C74" s="2">
         <v>1</v>
@@ -1739,7 +1734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E23FC18B-FD15-41B0-BC5E-FD4AB03FD270}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>